<commit_message>
接口问题汇总 Signed-off-by: qtongtek_xiongbin <xiongbin@qtongtek.com>
</commit_message>
<xml_diff>
--- a/文档/接口文档/接口问题汇总.xlsx
+++ b/文档/接口文档/接口问题汇总.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,42 +56,70 @@
     <t>出入证、用火、用电等接口</t>
   </si>
   <si>
+    <t>上传图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口问题描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>报建列表接口</t>
+  </si>
+  <si>
+    <t>最好那边能提供一个可以正确上传的图片和图片做过base64的结果给我们。我们好去调整参数。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解决方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://jsonapi.xxx.com?Method=&amp;Params=参数Json经Des加密后的字符串&amp;Sign=签名字符串，url还是按照这个格式来组成的吧，Params包含name就行了，图片的内容不用加密，只要把base64放在httpbody里面就行了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传的接口是要求图片用base64编码的。我们这边base64编码有选项要设置的。我们测试了下我们这边用base64各个参数都测试了下服务器都是不是一个json而是一个404的页面。后台测试：http://113.105.159.115:5030/test.aspx返回的是json {"verification":true,"total":1,"data":[{"state":0,"msg":"参数有误请检查参数合理性"}],"error":null}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传图片返回 "verification":true,"total":1,"data":[{"state":0,"msg":"参数有误请检查参数合理性"}],"error":null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>报建列表接口会额外再返回一个叫做“步骤”的返回参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>提交编辑申请的时候，返回json为{"verification":true,"total":0,"data":[],"error":null}，出入证没有返回cardId msg，用火也没有返回state msg字段，用电 也都是一样</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>上传图片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接口问题描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传图片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>报建列表接口</t>
-  </si>
-  <si>
-    <t>报建列表接口会额外再返回一个叫做“步骤”的返回参数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传的接口是要求图片用base64编码的。我们这边base64编码有选项要设置的。我们测试了下我们这边用base64各个参数都测试了下服务器都是不是一个json而是一个404的页面。后台测试：http://113.105.159.115:5030/test.aspx返回的是json {"verification":true,"total":1,"data":[{"state":0,"msg":"参数有误请检查参数合理性"}],"error":null}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最好那边能提供一个可以正确上传的图片和图片做过base64的结果给我们。我们好去调整参数。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>解决方法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://jsonapi.xxx.com?Method=&amp;Params=参数Json经Des加密后的字符串&amp;Sign=签名字符串，url还是按照这个格式来组成的吧，Params包含name就行了，图片的内容不用加密，只要把base64放在httpbody里面就行了</t>
+    <t>出入证申请</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口文档中描述的proposerId（用户id）应该填什么？查询出入证列表的数据并没有看到用户id的字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>proposerId（用户id） 当前登录用户id,登录时，获取到的用户信息包含uid该字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -138,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +185,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -171,9 +211,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -197,9 +236,29 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -502,132 +561,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="68.25" style="4" customWidth="1"/>
-    <col min="6" max="6" width="43.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.25" style="3" customWidth="1"/>
+    <col min="6" max="6" width="43.125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="10">
+        <v>41923</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="11" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="10">
+        <v>41925</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="19" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="18">
+        <v>41925</v>
+      </c>
+      <c r="B4" s="19">
+        <v>3</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="19" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="18">
+        <v>41925</v>
+      </c>
+      <c r="B5" s="19">
+        <v>4</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="E5" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="11" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A6" s="10">
+        <v>41925</v>
+      </c>
+      <c r="B6" s="11">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="7" t="s">
+      <c r="F6" s="13"/>
+      <c r="G6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A7" s="15">
+        <v>41925</v>
+      </c>
+      <c r="B7" s="16">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
-        <v>41923</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>41925</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
-        <v>41925</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
-        <v>41925</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="C7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>